<commit_message>
new conditions added, except routing
</commit_message>
<xml_diff>
--- a/queries.xlsx
+++ b/queries.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA20"/>
+  <dimension ref="A1:AA27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1774,10 +1774,8 @@
           <t>General Cargo</t>
         </is>
       </c>
-      <c r="X20" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
+      <c r="X20" t="n">
+        <v>21</v>
       </c>
       <c r="Y20" t="inlineStr"/>
       <c r="Z20" t="inlineStr">
@@ -1788,6 +1786,421 @@
       <c r="AA20" t="inlineStr">
         <is>
           <t>40ft</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr"/>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr"/>
+      <c r="O21" t="inlineStr"/>
+      <c r="P21" t="inlineStr"/>
+      <c r="Q21" t="inlineStr"/>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>QUOTE-20251213091212</t>
+        </is>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>nabeel</t>
+        </is>
+      </c>
+      <c r="T21" t="inlineStr">
+        <is>
+          <t>Karachi Port</t>
+        </is>
+      </c>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>Bandar Abbas</t>
+        </is>
+      </c>
+      <c r="V21" t="inlineStr">
+        <is>
+          <t>Food Item</t>
+        </is>
+      </c>
+      <c r="W21" t="inlineStr"/>
+      <c r="X21" t="n">
+        <v>12</v>
+      </c>
+      <c r="Y21" t="inlineStr"/>
+      <c r="Z21" t="inlineStr">
+        <is>
+          <t>2025-12-13 09:12:12</t>
+        </is>
+      </c>
+      <c r="AA21" t="inlineStr">
+        <is>
+          <t>Dry</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr"/>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr"/>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr"/>
+      <c r="O22" t="inlineStr"/>
+      <c r="P22" t="inlineStr"/>
+      <c r="Q22" t="inlineStr"/>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>QUOTE-20251213092116</t>
+        </is>
+      </c>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>nabeel</t>
+        </is>
+      </c>
+      <c r="T22" t="inlineStr">
+        <is>
+          <t>Karachi Port</t>
+        </is>
+      </c>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>Bandar Abbas Port</t>
+        </is>
+      </c>
+      <c r="V22" t="inlineStr">
+        <is>
+          <t>Food Item</t>
+        </is>
+      </c>
+      <c r="W22" t="inlineStr"/>
+      <c r="X22" t="n">
+        <v>123</v>
+      </c>
+      <c r="Y22" t="inlineStr"/>
+      <c r="Z22" t="inlineStr">
+        <is>
+          <t>2025-12-13 09:21:16</t>
+        </is>
+      </c>
+      <c r="AA22" t="inlineStr">
+        <is>
+          <t>Dry</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr"/>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr"/>
+      <c r="O23" t="inlineStr"/>
+      <c r="P23" t="inlineStr"/>
+      <c r="Q23" t="inlineStr"/>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>QUOTE-20251213100629</t>
+        </is>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>nabeel</t>
+        </is>
+      </c>
+      <c r="T23" t="inlineStr">
+        <is>
+          <t>Karachi Port</t>
+        </is>
+      </c>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>Bandar Abbas Port</t>
+        </is>
+      </c>
+      <c r="V23" t="inlineStr">
+        <is>
+          <t>Food Item</t>
+        </is>
+      </c>
+      <c r="W23" t="inlineStr"/>
+      <c r="X23" t="n">
+        <v>123</v>
+      </c>
+      <c r="Y23" t="inlineStr"/>
+      <c r="Z23" t="inlineStr">
+        <is>
+          <t>2025-12-13 10:06:29</t>
+        </is>
+      </c>
+      <c r="AA23" t="inlineStr">
+        <is>
+          <t>Dry</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr"/>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="inlineStr"/>
+      <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr"/>
+      <c r="M24" t="inlineStr"/>
+      <c r="N24" t="inlineStr"/>
+      <c r="O24" t="inlineStr"/>
+      <c r="P24" t="inlineStr"/>
+      <c r="Q24" t="inlineStr"/>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>QUOTE-20251213100836</t>
+        </is>
+      </c>
+      <c r="S24" t="inlineStr">
+        <is>
+          <t>nabeel</t>
+        </is>
+      </c>
+      <c r="T24" t="inlineStr">
+        <is>
+          <t>Karachi Port</t>
+        </is>
+      </c>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>Bandar Abbas Port</t>
+        </is>
+      </c>
+      <c r="V24" t="inlineStr">
+        <is>
+          <t>General Cargo</t>
+        </is>
+      </c>
+      <c r="W24" t="inlineStr"/>
+      <c r="X24" t="n">
+        <v>23</v>
+      </c>
+      <c r="Y24" t="inlineStr"/>
+      <c r="Z24" t="inlineStr">
+        <is>
+          <t>2025-12-13 10:08:36</t>
+        </is>
+      </c>
+      <c r="AA24" t="inlineStr">
+        <is>
+          <t>20ft Dry</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr"/>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="inlineStr"/>
+      <c r="K25" t="inlineStr"/>
+      <c r="L25" t="inlineStr"/>
+      <c r="M25" t="inlineStr"/>
+      <c r="N25" t="inlineStr"/>
+      <c r="O25" t="inlineStr"/>
+      <c r="P25" t="inlineStr"/>
+      <c r="Q25" t="inlineStr"/>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>QUOTE-20251213101827</t>
+        </is>
+      </c>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>nabeel</t>
+        </is>
+      </c>
+      <c r="T25" t="inlineStr">
+        <is>
+          <t>Karachi Port</t>
+        </is>
+      </c>
+      <c r="U25" t="inlineStr">
+        <is>
+          <t>Bandar Abbas Port</t>
+        </is>
+      </c>
+      <c r="V25" t="inlineStr">
+        <is>
+          <t>Food Item</t>
+        </is>
+      </c>
+      <c r="W25" t="inlineStr"/>
+      <c r="X25" t="n">
+        <v>1312</v>
+      </c>
+      <c r="Y25" t="inlineStr"/>
+      <c r="Z25" t="inlineStr">
+        <is>
+          <t>2025-12-13 10:18:27</t>
+        </is>
+      </c>
+      <c r="AA25" t="inlineStr">
+        <is>
+          <t>Dry</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr"/>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="inlineStr"/>
+      <c r="K26" t="inlineStr"/>
+      <c r="L26" t="inlineStr"/>
+      <c r="M26" t="inlineStr"/>
+      <c r="N26" t="inlineStr"/>
+      <c r="O26" t="inlineStr"/>
+      <c r="P26" t="inlineStr"/>
+      <c r="Q26" t="inlineStr"/>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>QUOTE-20251213101852</t>
+        </is>
+      </c>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>nabeel</t>
+        </is>
+      </c>
+      <c r="T26" t="inlineStr">
+        <is>
+          <t>Karachi Port</t>
+        </is>
+      </c>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>Bandar Abbas Port</t>
+        </is>
+      </c>
+      <c r="V26" t="inlineStr">
+        <is>
+          <t>General Cargo</t>
+        </is>
+      </c>
+      <c r="W26" t="inlineStr"/>
+      <c r="X26" t="n">
+        <v>12</v>
+      </c>
+      <c r="Y26" t="inlineStr"/>
+      <c r="Z26" t="inlineStr">
+        <is>
+          <t>2025-12-13 10:18:52</t>
+        </is>
+      </c>
+      <c r="AA26" t="inlineStr">
+        <is>
+          <t>Dry</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr"/>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr"/>
+      <c r="K27" t="inlineStr"/>
+      <c r="L27" t="inlineStr"/>
+      <c r="M27" t="inlineStr"/>
+      <c r="N27" t="inlineStr"/>
+      <c r="O27" t="inlineStr"/>
+      <c r="P27" t="inlineStr"/>
+      <c r="Q27" t="inlineStr"/>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>QUOTE-20251213103013</t>
+        </is>
+      </c>
+      <c r="S27" t="inlineStr">
+        <is>
+          <t>nabeel</t>
+        </is>
+      </c>
+      <c r="T27" t="inlineStr">
+        <is>
+          <t>Karachi Port</t>
+        </is>
+      </c>
+      <c r="U27" t="inlineStr">
+        <is>
+          <t>Bandar Abbas Port</t>
+        </is>
+      </c>
+      <c r="V27" t="inlineStr">
+        <is>
+          <t>General Cargo</t>
+        </is>
+      </c>
+      <c r="W27" t="inlineStr"/>
+      <c r="X27" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="Y27" t="inlineStr"/>
+      <c r="Z27" t="inlineStr">
+        <is>
+          <t>2025-12-13 10:30:13</t>
+        </is>
+      </c>
+      <c r="AA27" t="inlineStr">
+        <is>
+          <t>Dry</t>
         </is>
       </c>
     </row>

</xml_diff>